<commit_message>
added new words, fixed bug
</commit_message>
<xml_diff>
--- a/finnish.xlsx
+++ b/finnish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulin\PycharmProjects\learn_new_words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2097F1A-5B20-4BFD-A9B7-B09EC5D8B3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C4B2B-3007-46E2-B8CA-616AF9956570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7065" yWindow="990" windowWidth="21795" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2611,10 +2611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4087"/>
+  <dimension ref="A1:F4087"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D224" sqref="D224"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F249" sqref="F249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5273,7 +5273,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>60</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>298</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>173</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>174</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>175</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>299</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>273</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>176</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>177</v>
       </c>
@@ -5371,8 +5371,9 @@
       <c r="C249" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F249" s="2"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>337</v>
       </c>
@@ -5383,7 +5384,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>87</v>
       </c>
@@ -5394,7 +5395,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>300</v>
       </c>
@@ -5405,7 +5406,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>338</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>178</v>
       </c>
@@ -5427,7 +5428,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>179</v>
       </c>
@@ -5438,7 +5439,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
class now being displayed
</commit_message>
<xml_diff>
--- a/finnish.xlsx
+++ b/finnish.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulin\PycharmProjects\learn_new_words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C4B2B-3007-46E2-B8CA-616AF9956570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B98B43-EFC8-4F99-A9DC-F1436E8CC1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="990" windowWidth="21795" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5970" yWindow="3135" windowWidth="21795" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2613,8 +2613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4087"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F249" sqref="F249"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E270" sqref="E270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5450,7 +5450,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>158</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>3</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>181</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>301</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>302</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>182</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>183</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>207</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>95</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>4</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>184</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>5</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>185</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>128</v>
       </c>
@@ -5603,8 +5603,9 @@
       <c r="C270" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E270" s="2"/>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>107</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>339</v>
       </c>

</xml_diff>